<commit_message>
fixed decomp, I think
</commit_message>
<xml_diff>
--- a/output/out_2023-10-30T14:19:55.787/decompositions/decompositions_combined.xlsx
+++ b/output/out_2023-10-30T14:19:55.787/decompositions/decompositions_combined.xlsx
@@ -406,7 +406,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -444,6 +444,70 @@
         <v>9</v>
       </c>
     </row>
+    <row r="2" spans="1:10">
+      <c r="A2">
+        <v>54</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0.021158669831225007</v>
+      </c>
+      <c r="D2">
+        <v>0.016484502794454983</v>
+      </c>
+      <c r="E2">
+        <v>0.01968222822834191</v>
+      </c>
+      <c r="F2">
+        <v>0.018181902261260527</v>
+      </c>
+      <c r="G2">
+        <v>0.3158726659249553</v>
+      </c>
+      <c r="H2">
+        <v>0.6841273340750447</v>
+      </c>
+      <c r="I2">
+        <v>0.6368551972035442</v>
+      </c>
+      <c r="J2">
+        <v>0.3631448027964557</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4">
+        <v>56</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0.016745579186857058</v>
+      </c>
+      <c r="D4">
+        <v>0.02706542569107139</v>
+      </c>
+      <c r="E4">
+        <v>0.022720558189598034</v>
+      </c>
+      <c r="F4">
+        <v>0.020430256127836888</v>
+      </c>
+      <c r="G4">
+        <v>0.578979445120716</v>
+      </c>
+      <c r="H4">
+        <v>0.42102055487928397</v>
+      </c>
+      <c r="I4">
+        <v>0.3570476498342405</v>
+      </c>
+      <c r="J4">
+        <v>0.6429523501657596</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>